<commit_message>
ROSES form as PDF - single page.
</commit_message>
<xml_diff>
--- a/Figures/Additional_files/Additional File 1_ROSES for Systematic Map Reports.xlsx
+++ b/Figures/Additional_files/Additional File 1_ROSES for Systematic Map Reports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrabl/Desktop/NS_review/Paper_publi/Paper_2/Figures/north_sea_review/Figures/Additional_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADF86AC-C542-7741-B4CF-EE3819AC332C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5C69D4-BA02-9145-8FBC-EC19CFE2D225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30840" yWindow="500" windowWidth="33000" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29200" yWindow="500" windowWidth="36940" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="163">
   <si>
     <t>ROSES for Systematic Map Reports. Version 1.0</t>
   </si>
@@ -566,6 +566,9 @@
   </si>
   <si>
     <t>Critical appraisal not performed</t>
+  </si>
+  <si>
+    <t>Google scholar search syntax</t>
   </si>
 </sst>
 </file>
@@ -668,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -712,9 +715,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1058,10 +1058,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2116,7 +2119,7 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup paperSize="9" scale="45" orientation="landscape"/>
 </worksheet>
 </file>
 
@@ -2124,12 +2127,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2344,7 +2346,7 @@
       <c r="F9" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="10" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2429,6 +2431,9 @@
       <c r="G13" t="s">
         <v>156</v>
       </c>
+      <c r="H13" s="10" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
@@ -2445,7 +2450,7 @@
       <c r="F14" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="10" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2464,7 +2469,7 @@
       <c r="F15" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="10" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2530,7 +2535,7 @@
       <c r="G18" s="10">
         <v>7</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="19" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2804,7 +2809,7 @@
       <c r="F31" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="21">
+      <c r="G31" s="20">
         <v>32622</v>
       </c>
     </row>
@@ -2825,7 +2830,7 @@
       <c r="F32" t="s">
         <v>22</v>
       </c>
-      <c r="G32" s="21">
+      <c r="G32" s="20">
         <v>22511</v>
       </c>
     </row>
@@ -2865,7 +2870,7 @@
       <c r="F34" t="s">
         <v>22</v>
       </c>
-      <c r="G34" s="22" t="s">
+      <c r="G34" s="21" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2886,7 +2891,7 @@
       <c r="F35" t="s">
         <v>22</v>
       </c>
-      <c r="G35" s="19" t="s">
+      <c r="G35" s="10" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2907,7 +2912,7 @@
       <c r="F36" t="s">
         <v>22</v>
       </c>
-      <c r="G36" s="23">
+      <c r="G36" s="22">
         <v>7440</v>
       </c>
     </row>
@@ -2926,7 +2931,7 @@
       <c r="F37" t="s">
         <v>22</v>
       </c>
-      <c r="G37" s="23">
+      <c r="G37" s="22">
         <v>5795</v>
       </c>
     </row>
@@ -2945,7 +2950,7 @@
       <c r="F38" t="s">
         <v>28</v>
       </c>
-      <c r="G38" s="24" t="s">
+      <c r="G38" s="23" t="s">
         <v>146</v>
       </c>
     </row>
@@ -2964,7 +2969,7 @@
       <c r="F39" t="s">
         <v>22</v>
       </c>
-      <c r="G39" s="23">
+      <c r="G39" s="22">
         <v>3356</v>
       </c>
     </row>
@@ -9865,6 +9870,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup paperSize="9" scale="42" orientation="landscape"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rechecked files to be ready for submission (revision 2 - minor revisions)
</commit_message>
<xml_diff>
--- a/Figures/Additional_files/Additional File 1_ROSES for Systematic Map Reports.xlsx
+++ b/Figures/Additional_files/Additional File 1_ROSES for Systematic Map Reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrabl/Desktop/NS_review/Paper_publi/Paper_2/Figures/north_sea_review/Figures/Additional_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5C69D4-BA02-9145-8FBC-EC19CFE2D225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53376174-4ADD-8946-93B4-8C45D5A380B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29200" yWindow="500" windowWidth="36940" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,14 +568,14 @@
     <t>Critical appraisal not performed</t>
   </si>
   <si>
-    <t>Google scholar search syntax</t>
+    <t>Web of Science search syntax</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -640,13 +640,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -708,20 +702,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2131,7 +2127,9 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2172,967 +2170,1005 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="23" t="s">
         <v>152</v>
       </c>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
+      <c r="A3" s="21">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="17" t="s">
         <v>149</v>
       </c>
+      <c r="H3" s="17"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
+      <c r="A4" s="21">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" t="s">
+      <c r="E4" s="16"/>
+      <c r="F4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
+      <c r="A5" s="21">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" t="s">
+      <c r="E5" s="16"/>
+      <c r="F5" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
+      <c r="A6" s="21">
         <v>5</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H6" s="17"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9">
+      <c r="A7" s="21">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" t="s">
+      <c r="E7" s="16"/>
+      <c r="F7" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="16" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
+      <c r="A8" s="21">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9">
+      <c r="A9" s="21">
         <v>8</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="17" t="s">
         <v>154</v>
       </c>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
+      <c r="A10" s="21">
         <v>9</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="17" t="s">
         <v>155</v>
       </c>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
+      <c r="A11" s="21">
         <v>10</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" t="s">
+      <c r="E11" s="16"/>
+      <c r="F11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H11" s="17"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
+      <c r="A12" s="21">
         <v>11</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" t="s">
+      <c r="E12" s="16"/>
+      <c r="F12" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H12" s="17"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
+      <c r="A13" s="21">
         <v>12</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" t="s">
+      <c r="E13" s="16"/>
+      <c r="F13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="16" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9">
+      <c r="A14" s="21">
         <v>13</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10" t="s">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" t="s">
+      <c r="E14" s="16"/>
+      <c r="F14" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="16" t="s">
         <v>157</v>
       </c>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
+      <c r="A15" s="21">
         <v>14</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10" t="s">
+      <c r="B15" s="16"/>
+      <c r="C15" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" t="s">
+      <c r="E15" s="16"/>
+      <c r="F15" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="16" t="s">
         <v>157</v>
       </c>
+      <c r="H15" s="17"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
+      <c r="A16" s="21">
         <v>15</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10" t="s">
+      <c r="B16" s="16"/>
+      <c r="C16" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" t="s">
+      <c r="E16" s="16"/>
+      <c r="F16" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="16">
         <v>4</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="17" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
+      <c r="A17" s="21">
         <v>16</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10" t="s">
+      <c r="B17" s="16"/>
+      <c r="C17" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="10"/>
-      <c r="F17" t="s">
+      <c r="E17" s="16"/>
+      <c r="F17" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="16">
         <v>3</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="17" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
+      <c r="A18" s="21">
         <v>17</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10" t="s">
+      <c r="B18" s="16"/>
+      <c r="C18" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="F18" t="s">
+      <c r="E18" s="16"/>
+      <c r="F18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="16">
         <v>7</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="17" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9">
+      <c r="A19" s="21">
         <v>18</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" t="s">
+      <c r="E19" s="16"/>
+      <c r="F19" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H19" s="17"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9">
+      <c r="A20" s="21">
         <v>19</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10" t="s">
+      <c r="B20" s="16"/>
+      <c r="C20" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H20" s="17"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9">
+      <c r="A21" s="21">
         <v>20</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="F21" t="s">
+      <c r="E21" s="16"/>
+      <c r="F21" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H21" s="17"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9">
+      <c r="A22" s="21">
         <v>21</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10" t="s">
+      <c r="B22" s="16"/>
+      <c r="C22" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" t="s">
+      <c r="E22" s="16"/>
+      <c r="F22" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9">
+      <c r="A23" s="21">
         <v>22</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="16" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9">
+      <c r="A24" s="21">
         <v>23</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10" t="s">
+      <c r="B24" s="16"/>
+      <c r="C24" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="16" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9">
+      <c r="A25" s="21">
         <v>24</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="10"/>
-      <c r="F25" t="s">
+      <c r="E25" s="16"/>
+      <c r="F25" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="H25" s="10"/>
+      <c r="H25" s="16"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9">
+      <c r="A26" s="21">
         <v>25</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10" t="s">
+      <c r="B26" s="16"/>
+      <c r="C26" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" t="s">
+      <c r="E26" s="16"/>
+      <c r="F26" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H26" s="17"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9">
+      <c r="A27" s="21">
         <v>26</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" t="s">
+      <c r="E27" s="16"/>
+      <c r="F27" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H27" s="17"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9">
+      <c r="A28" s="21">
         <v>27</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10" t="s">
+      <c r="B28" s="16"/>
+      <c r="C28" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="10"/>
-      <c r="F28" t="s">
+      <c r="E28" s="16"/>
+      <c r="F28" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H28" s="17"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9">
+      <c r="A29" s="21">
         <v>28</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10" t="s">
+      <c r="B29" s="16"/>
+      <c r="C29" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H29" s="17"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9">
+      <c r="A30" s="21">
         <v>29</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="E30" s="10"/>
-      <c r="F30" t="s">
+      <c r="E30" s="16"/>
+      <c r="F30" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H30" s="17"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9">
+      <c r="A31" s="21">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10" t="s">
+      <c r="B31" s="16"/>
+      <c r="C31" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="20">
+      <c r="G31" s="22">
         <v>32622</v>
       </c>
+      <c r="H31" s="17"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9">
+      <c r="A32" s="21">
         <v>31</v>
       </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10" t="s">
+      <c r="B32" s="16"/>
+      <c r="C32" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G32" s="20">
+      <c r="G32" s="22">
         <v>22511</v>
       </c>
+      <c r="H32" s="17"/>
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9">
+      <c r="A33" s="21">
         <v>32</v>
       </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10" t="s">
+      <c r="B33" s="16"/>
+      <c r="C33" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="E33" s="10"/>
-      <c r="F33" t="s">
+      <c r="E33" s="16"/>
+      <c r="F33" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H33" s="17"/>
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9">
+      <c r="A34" s="21">
         <v>33</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10" t="s">
+      <c r="B34" s="16"/>
+      <c r="C34" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G34" s="21" t="s">
+      <c r="G34" s="18" t="s">
         <v>148</v>
       </c>
+      <c r="H34" s="17"/>
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9">
+      <c r="A35" s="21">
         <v>34</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10" t="s">
+      <c r="B35" s="16"/>
+      <c r="C35" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G35" s="10" t="s">
+      <c r="G35" s="16" t="s">
         <v>148</v>
       </c>
+      <c r="H35" s="17"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="9">
+      <c r="A36" s="21">
         <v>35</v>
       </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10" t="s">
+      <c r="B36" s="16"/>
+      <c r="C36" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G36" s="22">
+      <c r="G36" s="19">
         <v>7440</v>
       </c>
+      <c r="H36" s="20"/>
     </row>
     <row r="37" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="9">
+      <c r="A37" s="21">
         <v>36</v>
       </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10" t="s">
+      <c r="B37" s="16"/>
+      <c r="C37" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="E37" s="10"/>
-      <c r="F37" t="s">
+      <c r="E37" s="16"/>
+      <c r="F37" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G37" s="22">
+      <c r="G37" s="19">
         <v>5795</v>
       </c>
+      <c r="H37" s="20"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9">
+      <c r="A38" s="21">
         <v>37</v>
       </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10" t="s">
+      <c r="B38" s="16"/>
+      <c r="C38" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="E38" s="10"/>
-      <c r="F38" t="s">
+      <c r="E38" s="16"/>
+      <c r="F38" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G38" s="23" t="s">
+      <c r="G38" s="20" t="s">
         <v>146</v>
       </c>
+      <c r="H38" s="20"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9">
+      <c r="A39" s="21">
         <v>38</v>
       </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10" t="s">
+      <c r="B39" s="16"/>
+      <c r="C39" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="E39" s="10"/>
-      <c r="F39" t="s">
+      <c r="E39" s="16"/>
+      <c r="F39" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G39" s="22">
+      <c r="G39" s="19">
         <v>3356</v>
       </c>
+      <c r="H39" s="20"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="9">
+      <c r="A40" s="21">
         <v>39</v>
       </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10" t="s">
+      <c r="B40" s="16"/>
+      <c r="C40" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D40" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E40" s="10"/>
-      <c r="F40" t="s">
+      <c r="E40" s="16"/>
+      <c r="F40" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H40" s="17"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="9">
+      <c r="A41" s="21">
         <v>40</v>
       </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10" t="s">
+      <c r="B41" s="16"/>
+      <c r="C41" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D41" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E41" s="10"/>
-      <c r="F41" t="s">
+      <c r="E41" s="16"/>
+      <c r="F41" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H41" s="17"/>
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="9">
+      <c r="A42" s="21">
         <v>41</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10" t="s">
+      <c r="B42" s="16"/>
+      <c r="C42" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="E42" s="10"/>
-      <c r="F42" t="s">
+      <c r="E42" s="16"/>
+      <c r="F42" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H42" s="17"/>
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="9">
+      <c r="A43" s="21">
         <v>42</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10" t="s">
+      <c r="B43" s="16"/>
+      <c r="C43" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E43" s="10"/>
-      <c r="F43" t="s">
+      <c r="E43" s="16"/>
+      <c r="F43" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H43" s="17"/>
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="9">
+      <c r="A44" s="21">
         <v>43</v>
       </c>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10" t="s">
+      <c r="B44" s="16"/>
+      <c r="C44" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="E44" s="10"/>
-      <c r="F44" t="s">
+      <c r="E44" s="16"/>
+      <c r="F44" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H44" s="17"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="9">
+      <c r="A45" s="21">
         <v>44</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D45" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="E45" s="10"/>
-      <c r="F45" t="s">
+      <c r="E45" s="16"/>
+      <c r="F45" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G45" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H45" s="17"/>
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="9">
+      <c r="A46" s="21">
         <v>45</v>
       </c>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10" t="s">
+      <c r="B46" s="16"/>
+      <c r="C46" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G46" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H46" s="17"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="9">
+      <c r="A47" s="21">
         <v>46</v>
       </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10" t="s">
+      <c r="B47" s="16"/>
+      <c r="C47" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E47" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47" s="17" t="s">
         <v>146</v>
       </c>
+      <c r="H47" s="17"/>
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="9">
+      <c r="A48" s="21">
         <v>47</v>
       </c>
       <c r="B48" s="11" t="s">
@@ -3141,14 +3177,14 @@
       <c r="C48" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D48" s="16" t="s">
         <v>139</v>
       </c>
       <c r="E48" s="11"/>
       <c r="F48" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48" s="17" t="s">
         <v>146</v>
       </c>
       <c r="H48" s="11"/>

</xml_diff>